<commit_message>
WIP - Spreadsheet Loading Log
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/single_with_multiple_files_in_cell.xlsx
+++ b/storage/test_data/etl/single_with_multiple_files_in_cell.xlsx
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -171,10 +171,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.15"/>
@@ -185,7 +185,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="8.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="10.5"/>
   </cols>
@@ -263,7 +263,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>149.791951770446</v>
+        <v>133.933965586162</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>14</v>

</xml_diff>